<commit_message>
Atualizacao do arquivo de senha.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Matricula</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>084750mwca</t>
+  </si>
+  <si>
+    <t>cajuleda</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -683,7 +686,9 @@
       <c r="A17" s="2">
         <v>1610274</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">

</xml_diff>

<commit_message>
Tela de totalização das faltas
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Matricula</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>cajuleda</t>
+  </si>
+  <si>
+    <t>nairoterp167</t>
+  </si>
+  <si>
+    <t>0A@IPP7@0A</t>
   </si>
 </sst>
 </file>
@@ -121,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -138,6 +144,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,7 +573,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -642,7 +649,9 @@
       <c r="A10" s="6">
         <v>114210198</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="8">
+        <v>13058715</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
@@ -654,7 +663,9 @@
       <c r="A12" s="6">
         <v>115110163</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
@@ -680,7 +691,9 @@
       <c r="A16" s="6">
         <v>115110575</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">

</xml_diff>

<commit_message>
Primeiros testes do suporte a clustering com kMeans funcionando.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Matricula</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>ffc9507</t>
+  </si>
+  <si>
+    <t>L3d4-04081526</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -654,7 +657,9 @@
       <c r="A9" s="6">
         <v>112210079</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">

</xml_diff>

<commit_message>
Atualizacao com a senha de campelo
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Matricula</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>eclipse</t>
+  </si>
+  <si>
+    <t>dinossaur0</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -739,7 +742,9 @@
       <c r="A18" s="2">
         <v>2051962</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>

</xml_diff>

<commit_message>
Atualizacao das senhas (inclusao de Antonio Neto).
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Matricula</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>dinossaur0</t>
+  </si>
+  <si>
+    <t>Pedro%&amp;%&amp;5757q</t>
   </si>
 </sst>
 </file>
@@ -598,12 +601,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -632,7 +636,9 @@
       <c r="A4" s="6">
         <v>115111271</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">

</xml_diff>

<commit_message>
Atualizado arquivo de senhas para 2017.1
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,18 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Matricula</t>
   </si>
   <si>
     <t>Senha</t>
-  </si>
-  <si>
-    <t>jgyleda49</t>
-  </si>
-  <si>
-    <t>084750mwca</t>
   </si>
   <si>
     <t>cajuleda</t>
@@ -39,22 +33,7 @@
     <t>nairoterp167</t>
   </si>
   <si>
-    <t>0A@IPP7@0A</t>
-  </si>
-  <si>
-    <t>l3d@162</t>
-  </si>
-  <si>
-    <t>lcrleda13</t>
-  </si>
-  <si>
     <t>ffc9507</t>
-  </si>
-  <si>
-    <t>L3d4-04081526</t>
-  </si>
-  <si>
-    <t>eclipse</t>
   </si>
   <si>
     <t>dinossaur0</t>
@@ -62,12 +41,60 @@
   <si>
     <t>Pedro%&amp;%&amp;5757q</t>
   </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Antonio Pedro</t>
+  </si>
+  <si>
+    <t>Rafael Vieira</t>
+  </si>
+  <si>
+    <t>velmer</t>
+  </si>
+  <si>
+    <t>Valter Vinícius Marinho de Lucena</t>
+  </si>
+  <si>
+    <t>HIAGO NATAN FERNANDES DE SOUSA</t>
+  </si>
+  <si>
+    <t>Ivyna Rayany Santino Alves</t>
+  </si>
+  <si>
+    <t>Mateus Silva Luna</t>
+  </si>
+  <si>
+    <t>Ionesio Lima Da Costa Junior</t>
+  </si>
+  <si>
+    <t>José Glauber Braz de Oliveira</t>
+  </si>
+  <si>
+    <t>Camila Carvalho da Silva</t>
+  </si>
+  <si>
+    <t>Arthur Sampaio Perico Correia</t>
+  </si>
+  <si>
+    <t>Manuel Severino da Silva Neto</t>
+  </si>
+  <si>
+    <t>Dimitre Andrew Aires de Oliveira</t>
+  </si>
+  <si>
+    <t>Wesley Gonçalves Anibal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -102,6 +129,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -154,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -171,8 +204,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,11 +637,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1002"/>
+  <dimension ref="A1:C1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -610,188 +650,222 @@
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>115111901</v>
       </c>
       <c r="B2" s="7">
         <v>1029811465</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
-        <v>114110419</v>
-      </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>115111271</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
-        <v>115111271</v>
-      </c>
-      <c r="B4" s="8" t="s">
+        <v>113110905</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>115110575</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>115110671</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>116210587</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>115110295</v>
-      </c>
-      <c r="B5" s="7">
-        <v>87390509</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>114210779</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>115111033</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>114111359</v>
-      </c>
-      <c r="B8" s="7">
-        <v>31192510</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>112210079</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>114210198</v>
-      </c>
-      <c r="B10" s="8">
-        <v>13058715</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>114211200</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>115110163</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>115110721</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>114210695</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>113110905</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>115110575</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>115110057</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>113210626</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>115110120</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>115210873</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>115210195</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>115210213</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>114211270</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>113111794</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>115210629</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1610274</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2051962</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>2349850</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Modificacoes finais para colocar no ar para 2017.1.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Matricula</t>
   </si>
@@ -89,12 +89,24 @@
   <si>
     <t>Wesley Gonçalves Anibal</t>
   </si>
+  <si>
+    <t>senhadeleda</t>
+  </si>
+  <si>
+    <t>hiago060301</t>
+  </si>
+  <si>
+    <t>10450221Mila</t>
+  </si>
+  <si>
+    <t>Algorithm0!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -135,6 +147,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -187,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -211,6 +230,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -641,13 +665,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -698,7 +723,7 @@
       <c r="A5" s="6">
         <v>115110575</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -718,7 +743,9 @@
       <c r="A7" s="8">
         <v>116210587</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
@@ -727,7 +754,9 @@
       <c r="A8" s="8">
         <v>115110057</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="13">
+        <v>142754</v>
+      </c>
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
@@ -736,7 +765,9 @@
       <c r="A9" s="8">
         <v>113210626</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
@@ -763,7 +794,9 @@
       <c r="A12" s="8">
         <v>115210195</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
@@ -772,7 +805,9 @@
       <c r="A13" s="8">
         <v>115210213</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="C13" s="9" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Acrescentado mais senhas e id da planilah de EDA.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Matricula</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Algorithm0!</t>
+  </si>
+  <si>
+    <t>senhaleda</t>
+  </si>
+  <si>
+    <t>mnetinho</t>
   </si>
 </sst>
 </file>
@@ -665,7 +671,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -734,7 +740,9 @@
       <c r="A6" s="8">
         <v>115110671</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="13">
+        <v>81996</v>
+      </c>
       <c r="C6" s="9" t="s">
         <v>12</v>
       </c>
@@ -816,7 +824,9 @@
       <c r="A14" s="8">
         <v>114211270</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
@@ -825,7 +835,9 @@
       <c r="A15" s="8">
         <v>113111794</v>
       </c>
-      <c r="B15" s="9"/>
+      <c r="B15" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="C15" s="9" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Atualização das senhas e melhoria no reconhecimento da quantidade de turmas e de
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Matricula</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>mnetinho</t>
+  </si>
+  <si>
+    <t>jgbo1357</t>
   </si>
 </sst>
 </file>
@@ -671,7 +674,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -793,7 +796,9 @@
       <c r="A11" s="8">
         <v>115210873</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C11" s="9" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Atualizacao das senhas e do validador apra permitir download de roteiro de revisao antes do tempo.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Matricula</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Arthur Sampaio Perico Correia</t>
   </si>
   <si>
-    <t>Manuel Severino da Silva Neto</t>
-  </si>
-  <si>
     <t>Dimitre Andrew Aires de Oliveira</t>
   </si>
   <si>
@@ -105,17 +102,29 @@
     <t>senhaleda</t>
   </si>
   <si>
-    <t>mnetinho</t>
+    <t>jgbo1357</t>
   </si>
   <si>
-    <t>jgbo1357</t>
+    <t>ledamon2017</t>
+  </si>
+  <si>
+    <t>mel123456</t>
+  </si>
+  <si>
+    <t>wesleyolivedos</t>
+  </si>
+  <si>
+    <t>davi.nascimento@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>limao010203</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -163,6 +172,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -215,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -244,6 +259,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -674,7 +693,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -755,7 +774,7 @@
         <v>116210587</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>13</v>
@@ -777,7 +796,7 @@
         <v>113210626</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>15</v>
@@ -787,7 +806,9 @@
       <c r="A10" s="8">
         <v>115110120</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="C10" s="9" t="s">
         <v>16</v>
       </c>
@@ -797,7 +818,7 @@
         <v>115210873</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>17</v>
@@ -808,7 +829,7 @@
         <v>115210195</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>18</v>
@@ -819,21 +840,21 @@
         <v>115210213</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>114211270</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>20</v>
+      <c r="A14" s="15">
+        <v>115111577</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -841,19 +862,21 @@
         <v>113111794</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>115210629</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="C16" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -878,7 +901,9 @@
       <c r="A19" s="10">
         <v>2349850</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Pequenos ajustes no servidorpara linkar corretamente o arquivo de ambiente do roteiro especial
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Matricula</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>limao010203</t>
+  </si>
+  <si>
+    <t>Lucas Arcoverde</t>
+  </si>
+  <si>
+    <t>lucas9835</t>
   </si>
 </sst>
 </file>
@@ -294,7 +300,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -337,7 +343,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -385,7 +391,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -689,11 +695,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1002"/>
+  <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -880,34 +886,42 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>1610274</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="3"/>
+      <c r="A17" s="8">
+        <v>115211049</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
+        <v>1610274</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>2051962</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
         <v>2349850</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
@@ -924,7 +938,7 @@
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -3854,6 +3868,9 @@
     </row>
     <row r="1002" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1002" s="1"/>
+    </row>
+    <row r="1003" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1003" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajustados mais coisas no servidor para 2017.2
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Matricula</t>
   </si>
@@ -30,88 +30,13 @@
     <t>cajuleda</t>
   </si>
   <si>
-    <t>nairoterp167</t>
-  </si>
-  <si>
-    <t>ffc9507</t>
-  </si>
-  <si>
     <t>dinossaur0</t>
-  </si>
-  <si>
-    <t>Pedro%&amp;%&amp;5757q</t>
-  </si>
-  <si>
-    <t>Alice</t>
   </si>
   <si>
     <t>Nome</t>
   </si>
   <si>
-    <t>Antonio Pedro</t>
-  </si>
-  <si>
-    <t>Rafael Vieira</t>
-  </si>
-  <si>
-    <t>velmer</t>
-  </si>
-  <si>
-    <t>Valter Vinícius Marinho de Lucena</t>
-  </si>
-  <si>
-    <t>HIAGO NATAN FERNANDES DE SOUSA</t>
-  </si>
-  <si>
     <t>Ivyna Rayany Santino Alves</t>
-  </si>
-  <si>
-    <t>Mateus Silva Luna</t>
-  </si>
-  <si>
-    <t>Ionesio Lima Da Costa Junior</t>
-  </si>
-  <si>
-    <t>José Glauber Braz de Oliveira</t>
-  </si>
-  <si>
-    <t>Camila Carvalho da Silva</t>
-  </si>
-  <si>
-    <t>Arthur Sampaio Perico Correia</t>
-  </si>
-  <si>
-    <t>Dimitre Andrew Aires de Oliveira</t>
-  </si>
-  <si>
-    <t>Wesley Gonçalves Anibal</t>
-  </si>
-  <si>
-    <t>senhadeleda</t>
-  </si>
-  <si>
-    <t>hiago060301</t>
-  </si>
-  <si>
-    <t>10450221Mila</t>
-  </si>
-  <si>
-    <t>Algorithm0!</t>
-  </si>
-  <si>
-    <t>senhaleda</t>
-  </si>
-  <si>
-    <t>jgbo1357</t>
-  </si>
-  <si>
-    <t>ledamon2017</t>
-  </si>
-  <si>
-    <t>mel123456</t>
-  </si>
-  <si>
-    <t>wesleyolivedos</t>
   </si>
   <si>
     <t>davi.nascimento@ccc.ufcg.edu.br</t>
@@ -125,12 +50,45 @@
   <si>
     <t>lucas9835</t>
   </si>
+  <si>
+    <t>Antunes</t>
+  </si>
+  <si>
+    <t>Jose Robson</t>
+  </si>
+  <si>
+    <t>Marcos Williams</t>
+  </si>
+  <si>
+    <t>Hector</t>
+  </si>
+  <si>
+    <t>Italo</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Gabriel Valentino</t>
+  </si>
+  <si>
+    <t>Thalyta</t>
+  </si>
+  <si>
+    <t>Paulo Leitao</t>
+  </si>
+  <si>
+    <t>Jose Ivan</t>
+  </si>
+  <si>
+    <t>Joao Aristides</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -165,12 +123,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -236,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -259,18 +211,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,7 +249,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -343,7 +292,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -391,7 +340,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -695,11 +644,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1003"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -717,211 +666,167 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
-        <v>115111901</v>
+        <v>115110295</v>
       </c>
-      <c r="B2" s="7">
-        <v>1029811465</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
+      <c r="B2" s="7"/>
+      <c r="C2" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
-        <v>115111271</v>
+        <v>116110648</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
+      <c r="B3" s="7"/>
+      <c r="C3" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
-        <v>113110905</v>
+        <v>114210695</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
+      <c r="B4" s="7"/>
+      <c r="C4" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>115110575</v>
+        <v>115210859</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
+      <c r="B5" s="7"/>
+      <c r="C5" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
-        <v>115110671</v>
+        <v>115111014</v>
       </c>
-      <c r="B6" s="13">
-        <v>81996</v>
-      </c>
+      <c r="B6" s="11"/>
       <c r="C6" s="9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
-        <v>116210587</v>
+        <v>116111420</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="B7" s="12"/>
       <c r="C7" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>115110057</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>142754</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
-        <v>113210626</v>
+        <v>115210052</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="B9" s="7"/>
       <c r="C9" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
-        <v>115110120</v>
+        <v>115210685</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>28</v>
-      </c>
+      <c r="B10" s="7"/>
       <c r="C10" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
-        <v>115210873</v>
+        <v>116110175</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="B11" s="7"/>
       <c r="C11" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
-        <v>115210195</v>
+        <v>115210700</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>24</v>
-      </c>
+      <c r="B12" s="7"/>
       <c r="C12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
-        <v>115210213</v>
+        <v>114210797</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>22</v>
+      <c r="B13" s="7"/>
+      <c r="C13" s="9" t="s">
+        <v>20</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15">
+      <c r="A14" s="13">
         <v>115111577</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
-        <v>113111794</v>
+        <v>115211049</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>26</v>
+      <c r="B15" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>115210629</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
-        <v>115211049</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A16" s="2">
         <v>1610274</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>2051962</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
+      <c r="B17" s="3" t="s">
+        <v>3</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
-        <v>2349850</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="3"/>
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
@@ -932,13 +837,13 @@
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -3862,15 +3767,6 @@
     </row>
     <row r="1000" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1000" s="1"/>
-    </row>
-    <row r="1001" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1001" s="1"/>
-    </row>
-    <row r="1002" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1002" s="1"/>
-    </row>
-    <row r="1003" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1003" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Atualizacao do pom do plugin de correcao.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Senhas.xlsx
+++ b/leda-submission-server/conf/Senhas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Matricula</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>davi.nascimento@ccc.ufcg.edu.br</t>
-  </si>
-  <si>
-    <t>limao010203</t>
   </si>
   <si>
     <t>Lucas Arcoverde</t>
@@ -83,12 +80,36 @@
   <si>
     <t>Joao Aristides</t>
   </si>
+  <si>
+    <t>lwymmd13121989</t>
+  </si>
+  <si>
+    <t>marcoswca1@</t>
+  </si>
+  <si>
+    <t>leda1313</t>
+  </si>
+  <si>
+    <t>gvba1996</t>
+  </si>
+  <si>
+    <t>pj97ebl02</t>
+  </si>
+  <si>
+    <t>campinense1</t>
+  </si>
+  <si>
+    <t>thelordoftherings</t>
+  </si>
+  <si>
+    <t>limao011</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,13 +144,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -215,11 +229,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,7 +662,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -673,54 +687,66 @@
       <c r="A2" s="6">
         <v>115110295</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="11">
+        <v>87390509</v>
+      </c>
       <c r="C2" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>116110648</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>114210695</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>115210859</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>115111014</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="11">
+        <v>99177192</v>
+      </c>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>116111420</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11">
+        <v>917253</v>
+      </c>
       <c r="C7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -728,7 +754,7 @@
         <v>115110057</v>
       </c>
       <c r="B8" s="11">
-        <v>142754</v>
+        <v>142854</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>5</v>
@@ -738,55 +764,65 @@
       <c r="A9" s="8">
         <v>115210052</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>115210685</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="11">
+        <v>312589</v>
+      </c>
       <c r="C10" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>116110175</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="C11" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>115210700</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>114210797</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
+      <c r="A14" s="12">
         <v>115111577</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -795,10 +831,10 @@
         <v>115211049</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>